<commit_message>
Updating Person Classification evaluation directory with latest confusion matrices and results
</commit_message>
<xml_diff>
--- a/evaluation/facial_rec/results/video_1/results.xlsx
+++ b/evaluation/facial_rec/results/video_1/results.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvass\Documents\FYP\Code\evaluation\facial_rec\results\video_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484671B8-FEBC-4077-9B61-8D96EB45FCB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77AE8D8-97E0-4C24-A220-A5C40C5875F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ArcFace" sheetId="1" r:id="rId1"/>
+    <sheet name="VGGFace" sheetId="2" r:id="rId2"/>
+    <sheet name="FaceNet512" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,14 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
   <si>
     <t>Metric</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
     <t>Accuracy</t>
   </si>
   <si>
@@ -43,6 +42,15 @@
   </si>
   <si>
     <t>F1-Score</t>
+  </si>
+  <si>
+    <t>Value (Weighted)</t>
+  </si>
+  <si>
+    <t>Value (Micro)</t>
+  </si>
+  <si>
+    <t>Value (Macro)</t>
   </si>
 </sst>
 </file>
@@ -360,58 +368,276 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2">
+        <v>0.99673400000000001</v>
+      </c>
+      <c r="C2">
+        <v>0.99673400000000001</v>
+      </c>
+      <c r="D2">
+        <v>0.99673400000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>0.99419000000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B3">
+        <v>0.99790699999999999</v>
+      </c>
+      <c r="C3">
+        <v>0.99673400000000001</v>
+      </c>
+      <c r="D3">
+        <v>0.79874500000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>0.99393299999999996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B4">
+        <v>0.99673400000000001</v>
+      </c>
+      <c r="C4">
+        <v>0.99673400000000001</v>
+      </c>
+      <c r="D4">
+        <v>0.99745200000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>0.99419000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
       <c r="B5">
-        <v>0.99388299999999996</v>
+        <v>0.99715200000000004</v>
+      </c>
+      <c r="C5">
+        <v>0.99673400000000001</v>
+      </c>
+      <c r="D5">
+        <v>0.85524</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0940C78-2B9C-454F-81F6-A1B4E9BB2864}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.99738700000000002</v>
+      </c>
+      <c r="C2">
+        <v>0.99738700000000002</v>
+      </c>
+      <c r="D2">
+        <v>0.99738700000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.99912900000000004</v>
+      </c>
+      <c r="C3">
+        <v>0.99738700000000002</v>
+      </c>
+      <c r="D3">
+        <v>0.77777799999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.99738700000000002</v>
+      </c>
+      <c r="C4">
+        <v>0.99738700000000002</v>
+      </c>
+      <c r="D4">
+        <v>0.99749399999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.99803600000000003</v>
+      </c>
+      <c r="C5">
+        <v>0.99738700000000002</v>
+      </c>
+      <c r="D5">
+        <v>0.83207500000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D345FBFD-A53F-4F8F-9349-1847087FEAD8}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.99738700000000002</v>
+      </c>
+      <c r="C2">
+        <v>0.99738700000000002</v>
+      </c>
+      <c r="D2">
+        <v>0.99738700000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.99912900000000004</v>
+      </c>
+      <c r="C3">
+        <v>0.99738700000000002</v>
+      </c>
+      <c r="D3">
+        <v>0.77777799999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.99738700000000002</v>
+      </c>
+      <c r="C4">
+        <v>0.99738700000000002</v>
+      </c>
+      <c r="D4">
+        <v>0.99749399999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.99803600000000003</v>
+      </c>
+      <c r="C5">
+        <v>0.99738700000000002</v>
+      </c>
+      <c r="D5">
+        <v>0.83207500000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>